<commit_message>
Final version submitted to ESTIMedia (figure file type changes)
</commit_message>
<xml_diff>
--- a/RawImages/Workbook1.xlsx
+++ b/RawImages/Workbook1.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23206"/>
-  <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23416"/>
+  <workbookPr showInkAnnotation="0" checkCompatibility="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="23480" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Chart1" sheetId="3" r:id="rId1"/>
@@ -886,11 +886,11 @@
         </c:dLbls>
         <c:gapWidth val="95"/>
         <c:overlap val="100"/>
-        <c:axId val="2119049080"/>
-        <c:axId val="2118416584"/>
+        <c:axId val="2118408488"/>
+        <c:axId val="2118411496"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2119049080"/>
+        <c:axId val="2118408488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -909,7 +909,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2118416584"/>
+        <c:crossAx val="2118411496"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -917,7 +917,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2118416584"/>
+        <c:axId val="2118411496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="65536.0"/>
@@ -929,7 +929,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2119049080"/>
+        <c:crossAx val="2118408488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="4086.0"/>
@@ -1553,11 +1553,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2143259976"/>
-        <c:axId val="2119772504"/>
+        <c:axId val="2117142616"/>
+        <c:axId val="2117139352"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="-2143259976"/>
+        <c:axId val="2117142616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1572,7 +1572,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="2119772504"/>
+        <c:crossAx val="2117139352"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1580,7 +1580,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2119772504"/>
+        <c:axId val="2117139352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1591,7 +1591,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2143259976"/>
+        <c:crossAx val="2117142616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1.0"/>
@@ -1928,11 +1928,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="-2143151992"/>
-        <c:axId val="2132190120"/>
+        <c:axId val="2117103880"/>
+        <c:axId val="2117100808"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2143151992"/>
+        <c:axId val="2117103880"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1942,7 +1942,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2132190120"/>
+        <c:crossAx val="2117100808"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1950,7 +1950,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2132190120"/>
+        <c:axId val="2117100808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="41363.0"/>
@@ -1963,7 +1963,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2143151992"/>
+        <c:crossAx val="2117103880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1984,7 +1984,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="182" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="102" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
@@ -1996,7 +1996,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9341093" cy="6648415"/>
+    <xdr:ext cx="9811373" cy="6985000"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -2248,8 +2248,8 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>

</xml_diff>